<commit_message>
fix(publipostage): Correct status, status name, status label ...
</commit_message>
<xml_diff>
--- a/publipostage2/004dan487/liste_essais_cliniques_identifies_004dan487.xlsx
+++ b/publipostage2/004dan487/liste_essais_cliniques_identifies_004dan487.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
   <si>
     <t>statut</t>
   </si>
   <si>
-    <t>statut_label</t>
-  </si>
-  <si>
     <t>statut_name</t>
   </si>
   <si>
@@ -43,52 +40,31 @@
     <t>acronym</t>
   </si>
   <si>
-    <t>results_1y</t>
-  </si>
-  <si>
-    <t>results_3y</t>
-  </si>
-  <si>
-    <t>results</t>
-  </si>
-  <si>
     <t>intervention_type</t>
   </si>
   <si>
-    <t>-3</t>
-  </si>
-  <si>
-    <t>⚠️</t>
-  </si>
-  <si>
-    <t>✅</t>
-  </si>
-  <si>
-    <t>+3</t>
-  </si>
-  <si>
-    <t>rouge</t>
-  </si>
-  <si>
-    <t>noir</t>
-  </si>
-  <si>
-    <t>vert</t>
-  </si>
-  <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>résultat postés ou publiés</t>
-  </si>
-  <si>
-    <t>pas de résultat postés ni publiés</t>
-  </si>
-  <si>
-    <t>résultat postés ou publiés dans les 12 mois</t>
-  </si>
-  <si>
-    <t>résultat postés ou publiés dans les 36 mois</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3: résultats postés ou publiés après les 36 mois</t>
+  </si>
+  <si>
+    <t>4: pas de résultats postés ni publiés</t>
+  </si>
+  <si>
+    <t>1: résultats postés ou publiés dans les 12 mois</t>
+  </si>
+  <si>
+    <t>2: résultats postés ou publiés entre 12 et 36 mois</t>
   </si>
   <si>
     <t>NCT00551551</t>
@@ -665,13 +641,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,679 +675,439 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
+      <c r="F6" t="s">
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
-      </c>
-      <c r="J6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
       <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="I8" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
-      </c>
-      <c r="J9" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" t="b">
-        <v>1</v>
-      </c>
-      <c r="L9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
       <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>81</v>
-      </c>
-      <c r="J10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
       <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
-      </c>
-      <c r="J11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" t="b">
-        <v>1</v>
-      </c>
-      <c r="L11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
       <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
       <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="I13" t="s">
         <v>84</v>
       </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
       <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H14" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="I14" t="s">
-        <v>85</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
       <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="I15" t="s">
-        <v>86</v>
-      </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
       <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="I16" t="s">
-        <v>87</v>
-      </c>
-      <c r="J16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
       <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I17" t="s">
-        <v>88</v>
-      </c>
-      <c r="J17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" t="b">
-        <v>0</v>
-      </c>
-      <c r="M17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
       <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
       </c>
       <c r="G18" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="I18" t="s">
         <v>89</v>
       </c>
-      <c r="J18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" t="b">
-        <v>0</v>
-      </c>
-      <c r="M18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
       <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
       </c>
       <c r="G19" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="H19" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="I19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="b">
-        <v>0</v>
-      </c>
-      <c r="L19" t="b">
-        <v>0</v>
-      </c>
-      <c r="M19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
       <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" t="b">
-        <v>0</v>
-      </c>
-      <c r="M20" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>